<commit_message>
GRESB and City LEED
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
+++ b/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3677" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="1129">
   <si>
     <t>ProjectName</t>
   </si>
@@ -3450,6 +3450,18 @@
   </si>
   <si>
     <t>1000163195</t>
+  </si>
+  <si>
+    <t>USCityNone 15:05:51</t>
+  </si>
+  <si>
+    <t>9000116523</t>
+  </si>
+  <si>
+    <t>Apr 18, 2019</t>
+  </si>
+  <si>
+    <t>1000087736</t>
   </si>
 </sst>
 </file>
@@ -14853,7 +14865,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="25.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="25.9140625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="26" width="14.140625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="26" width="25.7109375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
@@ -14872,7 +14884,7 @@
     <col min="18" max="18" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
     <col min="19" max="19" customWidth="true" style="26" width="36.5703125" collapsed="true"/>
     <col min="20" max="20" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="26" width="13.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="26" width="13.26171875" collapsed="true"/>
     <col min="22" max="22" customWidth="true" style="26" width="12.85546875" collapsed="true"/>
     <col min="23" max="23" customWidth="true" style="26" width="17.140625" collapsed="true"/>
     <col min="24" max="24" customWidth="true" style="26" width="11.85546875" collapsed="true"/>
@@ -14894,7 +14906,7 @@
     <col min="41" max="41" customWidth="true" style="26" width="27.7109375" collapsed="true"/>
     <col min="42" max="42" width="9.140625" collapsed="true"/>
     <col min="43" max="43" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="26" width="12.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="26" width="12.78515625" collapsed="true"/>
     <col min="45" max="45" customWidth="true" style="26" width="39.28515625" collapsed="true"/>
     <col min="46" max="46" customWidth="true" style="26" width="12.5703125" collapsed="true"/>
     <col min="47" max="47" customWidth="true" style="26" width="19.7109375" collapsed="true"/>
@@ -15406,7 +15418,7 @@
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>1092</v>
+        <v>1125</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>353</v>
@@ -15454,7 +15466,7 @@
         <v>397</v>
       </c>
       <c r="U4" s="55" t="s">
-        <v>1093</v>
+        <v>1128</v>
       </c>
       <c r="V4" s="52" t="s">
         <v>260</v>
@@ -15506,7 +15518,7 @@
         <v>90</v>
       </c>
       <c r="AR4" t="s">
-        <v>1094</v>
+        <v>1127</v>
       </c>
       <c r="AS4" s="73" t="s">
         <v>123</v>

</xml_diff>

<commit_message>
City comm suite dev
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
+++ b/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21628"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KatalonProject\Automation\Automation\ARCDataTemplete\"/>
     </mc:Choice>
@@ -38,7 +38,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4168" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4171" uniqueCount="1142">
   <si>
     <t>ProjectName</t>
   </si>
@@ -3471,6 +3471,15 @@
   </si>
   <si>
     <t>1000145542</t>
+  </si>
+  <si>
+    <t>USCityLEED v4.1 12:49:29</t>
+  </si>
+  <si>
+    <t>1000145712</t>
+  </si>
+  <si>
+    <t>Apr 30, 2019</t>
   </si>
 </sst>
 </file>
@@ -4473,64 +4482,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="19" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="13" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="14" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="27" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="6.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="55" max="55" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="58" max="58" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="60" max="60" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="61" max="61" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="23.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68">
@@ -5870,12 +5879,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="101.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="101.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65">
@@ -6951,47 +6960,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="84" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="9.140625" style="84" collapsed="1"/>
-    <col min="16" max="16" width="12.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.140625" style="84" collapsed="1"/>
-    <col min="18" max="18" width="20" style="84" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="9.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="8.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15" style="84" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="11.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5703125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="11.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="15.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="62" width="9.140625" style="84" collapsed="1"/>
-    <col min="63" max="63" width="25.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="64" max="67" width="9.140625" style="84" collapsed="1"/>
-    <col min="68" max="68" width="16.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="9.140625" style="84" collapsed="1"/>
-    <col min="70" max="70" width="35.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="12" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="16" style="84" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" style="84" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="84" width="25.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="84" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="84" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="84" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="84" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" style="84" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="84" width="13.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="84" width="20.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="84" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="84" width="35.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="84" width="15.28515625" collapsed="true"/>
+    <col min="13" max="15" style="84" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="84" width="12.85546875" collapsed="true"/>
+    <col min="17" max="17" style="84" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="84" width="20.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="84" width="9.85546875" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" style="84" width="8.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="84" width="13.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="84" width="10.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="84" width="11.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="84" width="15.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="84" width="8.5703125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="84" width="8.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="84" width="14.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="84" width="12.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="84" width="14.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="84" width="17.28515625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="36" max="62" style="84" width="9.140625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" style="84" width="25.7109375" collapsed="true"/>
+    <col min="64" max="67" style="84" width="9.140625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" style="84" width="16.5703125" collapsed="true"/>
+    <col min="69" max="69" style="84" width="9.140625" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" style="84" width="35.85546875" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" style="84" width="12.0" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" style="84" width="16.0" collapsed="true"/>
+    <col min="73" max="16384" style="84" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73">
@@ -8652,43 +8661,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="40.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.140625" style="84" collapsed="1"/>
-    <col min="17" max="17" width="20" style="84" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="7.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.140625" style="84" collapsed="1"/>
-    <col min="24" max="24" width="11.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7" style="84" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.140625" style="84" collapsed="1"/>
-    <col min="27" max="27" width="14.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="11.5703125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="14.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="17.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="70" width="9.140625" style="84" collapsed="1"/>
-    <col min="71" max="71" width="13.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" style="84" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="84" width="25.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="84" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="84" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="84" width="17.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="84" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="84" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="84" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="84" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="84" width="40.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="84" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="84" width="12.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="84" width="16.28515625" collapsed="true"/>
+    <col min="16" max="16" style="84" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="84" width="20.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="84" width="9.5703125" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="84" width="7.7109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="84" width="10.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="84" width="13.42578125" collapsed="true"/>
+    <col min="23" max="23" style="84" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="84" width="7.0" collapsed="true"/>
+    <col min="26" max="26" style="84" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="84" width="14.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="84" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="84" width="14.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="84" width="17.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="84" width="22.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="35" max="70" style="84" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="84" width="13.140625" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="73" max="16384" style="84" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -10319,22 +10328,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75">
@@ -10652,25 +10661,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23" style="47" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" style="47" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" style="47" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="47" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="47" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="47" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="47" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="9.140625" style="47" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="9.140625" style="47" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" style="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="36.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.7109375" style="47" customWidth="1" collapsed="1"/>
-    <col min="22" max="16384" width="9.140625" style="47" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="47" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="47" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="47" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="47" width="24.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="47" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="47" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="47" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="47" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="47" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="47" width="15.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="47" width="14.42578125" collapsed="true"/>
+    <col min="13" max="14" style="47" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="47" width="13.140625" collapsed="true"/>
+    <col min="16" max="17" style="47" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="47" width="9.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="47" width="36.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="47" width="12.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="47" width="12.7109375" collapsed="true"/>
+    <col min="22" max="16384" style="47" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="31.5">
@@ -11002,17 +11011,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" style="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21" style="35" customWidth="1" collapsed="1"/>
-    <col min="6" max="10" width="9.140625" style="35" collapsed="1"/>
-    <col min="11" max="11" width="13.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="35" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="9.140625" style="35" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="35" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="35" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="35" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="35" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="35" width="21.0" collapsed="true"/>
+    <col min="6" max="10" style="35" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="35" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="35" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="35" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="35" width="21.7109375" collapsed="true"/>
+    <col min="15" max="16384" style="35" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -11313,26 +11322,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" style="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" style="32" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.28515625" style="32" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21" style="32" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" style="32" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="32" collapsed="1"/>
-    <col min="10" max="10" width="31.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="32" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="32" collapsed="1"/>
-    <col min="14" max="14" width="12.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5703125" style="32" customWidth="1" collapsed="1"/>
-    <col min="16" max="28" width="9.140625" style="32" collapsed="1"/>
-    <col min="29" max="29" width="12.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="30" max="38" width="9.140625" style="32" collapsed="1"/>
-    <col min="39" max="39" width="18.5703125" style="32" customWidth="1" collapsed="1"/>
-    <col min="40" max="16384" width="9.140625" style="32" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="32" width="17.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="32" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="32" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="32" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="32" width="21.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="32" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="32" width="21.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="32" width="18.0" collapsed="true"/>
+    <col min="9" max="9" style="32" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="32" width="31.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="32" width="12.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="32" width="10.85546875" collapsed="true"/>
+    <col min="13" max="13" style="32" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="32" width="12.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="32" width="15.5703125" collapsed="true"/>
+    <col min="16" max="28" style="32" width="9.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="32" width="12.7109375" collapsed="true"/>
+    <col min="30" max="38" style="32" width="9.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="32" width="18.5703125" collapsed="true"/>
+    <col min="40" max="16384" style="32" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
@@ -11976,26 +11985,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23" style="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="17" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="9.140625" style="17" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="9.140625" style="17" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="36.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="17" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="17" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="17" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="17" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="17" width="24.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="17" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="17" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="17" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="17" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="17" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="17" width="15.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="17" width="14.42578125" collapsed="true"/>
+    <col min="13" max="14" style="17" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="17" width="13.140625" collapsed="true"/>
+    <col min="16" max="17" style="17" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="17" width="9.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="17" width="36.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="17" width="14.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="17" width="16.42578125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="17" width="15.140625" collapsed="true"/>
+    <col min="23" max="16384" style="17" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="31.5">
@@ -12326,13 +12335,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75">
@@ -12650,49 +12659,49 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="23" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.140625" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.140625" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="23" width="9.140625" collapsed="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="27" width="9.140625" collapsed="1"/>
-    <col min="28" max="28" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="16" customWidth="1" collapsed="1"/>
-    <col min="33" max="37" width="9.140625" collapsed="1"/>
-    <col min="38" max="38" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="51" width="9.140625" collapsed="1"/>
-    <col min="52" max="52" width="23" customWidth="1" collapsed="1"/>
-    <col min="53" max="56" width="9.140625" collapsed="1"/>
-    <col min="57" max="57" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="58" max="61" width="9.140625" collapsed="1"/>
-    <col min="62" max="62" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="64" max="65" width="9.140625" collapsed="1"/>
-    <col min="66" max="66" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="9.140625" collapsed="1"/>
-    <col min="71" max="71" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="11" max="12" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="14" max="14" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="23" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="25" max="27" width="9.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="33" max="37" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="42" max="51" width="9.140625" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="53" max="56" width="9.140625" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="58" max="61" width="9.140625" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="64" max="65" width="9.140625" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="69" max="69" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="70" max="70" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="73" max="16384" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15.75">
@@ -13871,7 +13880,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -13931,22 +13940,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="35" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" style="35" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5703125" style="35" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="35" collapsed="1"/>
-    <col min="10" max="10" width="23.5703125" style="35" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="9.140625" style="35" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="35" customWidth="1" collapsed="1"/>
-    <col min="17" max="23" width="9.140625" style="35" collapsed="1"/>
-    <col min="24" max="24" width="12.42578125" style="35" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="9.140625" style="35" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="35" width="14.0" collapsed="true"/>
+    <col min="2" max="2" style="35" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="35" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="35" width="20.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="35" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="35" width="20.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="35" width="16.5703125" collapsed="true"/>
+    <col min="8" max="9" style="35" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="35" width="23.5703125" collapsed="true"/>
+    <col min="11" max="14" style="35" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="35" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="35" width="13.140625" collapsed="true"/>
+    <col min="17" max="23" style="35" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="35" width="12.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="35" width="20.85546875" collapsed="true"/>
+    <col min="26" max="16384" style="35" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -14315,23 +14324,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="27.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="9.140625" style="1" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="22" width="9.140625" style="1" collapsed="1"/>
-    <col min="23" max="23" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="8" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="27.42578125" collapsed="true"/>
+    <col min="11" max="14" style="1" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="18" max="22" style="1" width="9.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="25" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75">
@@ -14652,31 +14661,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="142" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="142" customWidth="1"/>
-    <col min="3" max="3" width="18" style="142" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="142"/>
-    <col min="5" max="5" width="20.140625" style="142" customWidth="1"/>
-    <col min="6" max="13" width="9.140625" style="142"/>
-    <col min="14" max="14" width="14.140625" style="142" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="142"/>
-    <col min="17" max="17" width="15.7109375" style="142" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="142"/>
-    <col min="19" max="19" width="13.140625" style="142" customWidth="1"/>
-    <col min="20" max="23" width="9.140625" style="142"/>
-    <col min="24" max="24" width="23.7109375" style="142" customWidth="1"/>
-    <col min="25" max="26" width="9.140625" style="142"/>
-    <col min="27" max="27" width="16.42578125" style="142" customWidth="1"/>
-    <col min="28" max="45" width="9.140625" style="142"/>
-    <col min="46" max="46" width="28.5703125" style="142" customWidth="1"/>
-    <col min="47" max="47" width="13.5703125" style="142" customWidth="1"/>
-    <col min="48" max="64" width="9.140625" style="142"/>
-    <col min="65" max="65" width="19.7109375" style="142" customWidth="1"/>
-    <col min="66" max="66" width="9.140625" style="142"/>
-    <col min="67" max="67" width="17.28515625" style="142" customWidth="1"/>
-    <col min="68" max="70" width="9.140625" style="142"/>
-    <col min="71" max="71" width="15.7109375" style="142" customWidth="1"/>
-    <col min="72" max="16384" width="9.140625" style="142"/>
+    <col min="1" max="1" customWidth="true" style="142" width="15.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="142" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="142" width="18.0" collapsed="true"/>
+    <col min="4" max="4" style="142" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="142" width="20.140625" collapsed="true"/>
+    <col min="6" max="13" style="142" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="142" width="14.140625" collapsed="true"/>
+    <col min="15" max="16" style="142" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="142" width="15.7109375" collapsed="true"/>
+    <col min="18" max="18" style="142" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="142" width="13.140625" collapsed="true"/>
+    <col min="20" max="23" style="142" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="142" width="23.7109375" collapsed="true"/>
+    <col min="25" max="26" style="142" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="142" width="16.42578125" collapsed="true"/>
+    <col min="28" max="45" style="142" width="9.140625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="142" width="28.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="142" width="13.5703125" collapsed="true"/>
+    <col min="48" max="64" style="142" width="9.140625" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" style="142" width="19.7109375" collapsed="true"/>
+    <col min="66" max="66" style="142" width="9.140625" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" style="142" width="17.28515625" collapsed="true"/>
+    <col min="68" max="70" style="142" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="142" width="15.7109375" collapsed="true"/>
+    <col min="72" max="16384" style="142" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -16800,8 +16809,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1">
@@ -17616,60 +17625,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="26" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="56.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.140625" style="26" collapsed="1"/>
-    <col min="17" max="17" width="16.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="14.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16" style="26" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="28.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="29.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="41.7109375" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="38.42578125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.42578125" style="72" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="40" width="9.140625" style="26" collapsed="1"/>
-    <col min="41" max="41" width="27.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="9.140625" collapsed="1"/>
-    <col min="43" max="43" width="20.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="19.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="39.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.5703125" style="26" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="19.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="49" max="50" width="21.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="18" style="26" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="20.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="22.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="20.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="17.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="19.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="57" max="16384" width="9.140625" style="26" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="25.9140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="26" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="26" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="26" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="26" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="26" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="26" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="26" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="26" width="56.7109375" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="26" width="14.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="26" width="20.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="26" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" style="26" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="26" width="16.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="26" width="24.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="26" width="12.484375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="26" width="12.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="26" width="17.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="26" width="11.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="26" width="15.28515625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="26" width="23.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="26" width="16.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="26" width="16.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="26" width="28.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="26" width="19.7109375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="26" width="22.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="26" width="29.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="41.7109375" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="72" width="12.42578125" collapsed="true"/>
+    <col min="39" max="40" style="26" width="9.140625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="26" width="27.7109375" collapsed="true"/>
+    <col min="42" max="42" width="9.140625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" style="26" width="13.58984375" collapsed="true" bestFit="true"/>
+    <col min="45" max="45" customWidth="true" style="26" width="39.28515625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="26" width="12.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="26" width="19.7109375" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="49" max="50" customWidth="true" style="26" width="21.85546875" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" style="26" width="18.0" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" style="26" width="20.42578125" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" style="26" width="22.42578125" collapsed="true"/>
+    <col min="54" max="54" customWidth="true" style="26" width="20.85546875" collapsed="true"/>
+    <col min="55" max="55" customWidth="true" style="26" width="17.85546875" collapsed="true"/>
+    <col min="56" max="56" customWidth="true" style="26" width="19.28515625" collapsed="true"/>
+    <col min="57" max="16384" style="26" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56">
@@ -17844,7 +17853,7 @@
     </row>
     <row r="2" spans="1:56">
       <c r="A2" s="52" t="s">
-        <v>360</v>
+        <v>1139</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>361</v>
@@ -17904,7 +17913,7 @@
         <v>370</v>
       </c>
       <c r="U2" s="58" t="s">
-        <v>371</v>
+        <v>1140</v>
       </c>
       <c r="V2" s="58" t="s">
         <v>267</v>
@@ -17973,7 +17982,7 @@
         <v>92</v>
       </c>
       <c r="AR2" s="138" t="s">
-        <v>382</v>
+        <v>1141</v>
       </c>
       <c r="AS2" s="26" t="s">
         <v>126</v>
@@ -18411,55 +18420,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="18" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="28.5703125" customWidth="1"/>
-    <col min="33" max="33" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="23.85546875" customWidth="1"/>
-    <col min="45" max="45" width="14.28515625" customWidth="1"/>
-    <col min="46" max="46" width="19" customWidth="1"/>
-    <col min="47" max="47" width="23.42578125" customWidth="1"/>
-    <col min="48" max="48" width="18.28515625" customWidth="1"/>
-    <col min="49" max="49" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="15.75">
@@ -19074,22 +19083,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="1" collapsed="1"/>
-    <col min="14" max="14" width="15.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="13" max="13" style="1" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="19" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -19630,10 +19639,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -19722,37 +19731,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.140625" collapsed="1"/>
-    <col min="15" max="15" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="16" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="14" max="14" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40">
@@ -20384,29 +20393,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="29" width="9.140625" style="1" collapsed="1"/>
-    <col min="30" max="30" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="20.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="26" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="9.140625" style="1" collapsed="1"/>
-    <col min="38" max="38" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="41" width="9.140625" style="1" collapsed="1"/>
-    <col min="42" max="42" width="15.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="11" max="29" style="1" width="9.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="20.140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="26.0" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="36" max="37" style="1" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="39" max="41" style="1" width="9.140625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="44" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43">

</xml_diff>

<commit_message>
Local Dev changes moved
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
+++ b/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
@@ -38,7 +38,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4168" uniqueCount="1139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4177" uniqueCount="1147">
   <si>
     <t>ProjectName</t>
   </si>
@@ -3471,6 +3471,30 @@
   </si>
   <si>
     <t>Apr 30, 2019</t>
+  </si>
+  <si>
+    <t>USCommOther 15:42:36</t>
+  </si>
+  <si>
+    <t>9000116412</t>
+  </si>
+  <si>
+    <t>1000145723</t>
+  </si>
+  <si>
+    <t>USCityLEED v4.1 16:52:46</t>
+  </si>
+  <si>
+    <t>USCityLEED v4.1 16:55:49</t>
+  </si>
+  <si>
+    <t>USCityLEED v4.1 17:04:49</t>
+  </si>
+  <si>
+    <t>USCityOther 17:06:33</t>
+  </si>
+  <si>
+    <t>9000116416</t>
   </si>
 </sst>
 </file>
@@ -3480,7 +3504,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4473,64 +4497,64 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="41" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="19" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="16" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="13" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="14" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="32.140625" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="27" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="28.85546875" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="35.28515625" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="41.140625" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="13" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="39.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" width="28.85546875" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="35.28515625" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
+    <col min="55" max="55" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="41.140625" collapsed="true"/>
+    <col min="58" max="58" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="59" max="59" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="60" max="60" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="61" max="61" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="23.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:68" x14ac:dyDescent="0.25">
@@ -5870,12 +5894,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="101.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="49" max="49" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="64" max="64" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="101.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" x14ac:dyDescent="0.25">
@@ -6951,47 +6975,47 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.140625" style="84" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="35.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="13" max="15" width="9.140625" style="84" collapsed="1"/>
-    <col min="16" max="16" width="12.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.140625" style="84" collapsed="1"/>
-    <col min="18" max="18" width="20" style="84" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="9.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="20" max="21" width="8.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="10.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15" style="84" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="12.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="11.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5703125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="14.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="11.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="15.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="62" width="9.140625" style="84" collapsed="1"/>
-    <col min="63" max="63" width="25.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="64" max="67" width="9.140625" style="84" collapsed="1"/>
-    <col min="68" max="68" width="16.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="9.140625" style="84" collapsed="1"/>
-    <col min="70" max="70" width="35.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="12" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="16" style="84" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" style="84" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="84" width="25.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="84" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="84" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="84" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="84" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" style="84" width="9.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="84" width="13.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="84" width="20.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="84" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="84" width="35.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="84" width="15.28515625" collapsed="true"/>
+    <col min="13" max="15" style="84" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="84" width="12.85546875" collapsed="true"/>
+    <col min="17" max="17" style="84" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="84" width="20.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="84" width="9.85546875" collapsed="true"/>
+    <col min="20" max="21" customWidth="true" style="84" width="8.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="84" width="13.85546875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="84" width="10.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="84" width="11.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="84" width="15.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="84" width="8.5703125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="84" width="8.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="84" width="14.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="84" width="12.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="84" width="14.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="84" width="17.28515625" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="36" max="62" style="84" width="9.140625" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" style="84" width="25.7109375" collapsed="true"/>
+    <col min="64" max="67" style="84" width="9.140625" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" style="84" width="16.5703125" collapsed="true"/>
+    <col min="69" max="69" style="84" width="9.140625" collapsed="true"/>
+    <col min="70" max="70" bestFit="true" customWidth="true" style="84" width="35.85546875" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" style="84" width="12.0" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" style="84" width="16.0" collapsed="true"/>
+    <col min="73" max="16384" style="84" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:73" x14ac:dyDescent="0.25">
@@ -8652,43 +8676,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="40.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.85546875" style="84" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.140625" style="84" collapsed="1"/>
-    <col min="17" max="17" width="20" style="84" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.5703125" style="84" customWidth="1" collapsed="1"/>
-    <col min="19" max="20" width="7.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="9.140625" style="84" collapsed="1"/>
-    <col min="24" max="24" width="11.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="7" style="84" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.140625" style="84" collapsed="1"/>
-    <col min="27" max="27" width="14.7109375" style="84" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="11.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="11.5703125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="14.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="17.28515625" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="22.42578125" style="84" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="15.42578125" style="84" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="70" width="9.140625" style="84" collapsed="1"/>
-    <col min="71" max="71" width="13.140625" style="84" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="11.28515625" style="84" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" style="84" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="84" width="25.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="84" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="84" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="84" width="17.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="84" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="84" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="84" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="84" width="19.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="84" width="40.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="84" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="84" width="12.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="84" width="16.28515625" collapsed="true"/>
+    <col min="16" max="16" style="84" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="84" width="20.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="84" width="9.5703125" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="84" width="7.7109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="84" width="10.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="84" width="13.42578125" collapsed="true"/>
+    <col min="23" max="23" style="84" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="84" width="7.0" collapsed="true"/>
+    <col min="26" max="26" style="84" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="84" width="14.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="84" width="12.28515625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="84" width="11.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="84" width="11.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="84" width="14.42578125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="84" width="17.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="84" width="22.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="84" width="15.42578125" collapsed="true"/>
+    <col min="35" max="70" style="84" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="84" width="13.140625" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" style="84" width="11.28515625" collapsed="true"/>
+    <col min="73" max="16384" style="84" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.25">
@@ -10319,22 +10343,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="11" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -10652,25 +10676,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="47" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" style="47" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" style="47" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="47" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="47" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="47" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="47" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="9.140625" style="47" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="9.140625" style="47" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" style="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="36.5703125" style="47" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.140625" style="47" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.7109375" style="47" customWidth="1" collapsed="1"/>
-    <col min="22" max="16384" width="9.140625" style="47" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="47" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="47" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="47" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="47" width="24.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="47" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="47" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="47" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="47" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="47" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="47" width="15.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="47" width="14.42578125" collapsed="true"/>
+    <col min="13" max="14" style="47" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="47" width="13.140625" collapsed="true"/>
+    <col min="16" max="17" style="47" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="47" width="9.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="47" width="36.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="47" width="12.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="47" width="12.7109375" collapsed="true"/>
+    <col min="22" max="16384" style="47" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
@@ -11002,17 +11026,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12" style="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21" style="35" customWidth="1" collapsed="1"/>
-    <col min="6" max="10" width="9.140625" style="35" collapsed="1"/>
-    <col min="11" max="11" width="13.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="19.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="35" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="15" max="16384" width="9.140625" style="35" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="35" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="35" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="35" width="18.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="35" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="35" width="21.0" collapsed="true"/>
+    <col min="6" max="10" style="35" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="35" width="13.85546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="35" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="35" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="35" width="21.7109375" collapsed="true"/>
+    <col min="15" max="16384" style="35" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -11313,26 +11337,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" style="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.42578125" style="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18" style="32" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.28515625" style="32" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="21" style="32" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18" style="32" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" style="32" collapsed="1"/>
-    <col min="10" max="10" width="31.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" style="32" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="32" collapsed="1"/>
-    <col min="14" max="14" width="12.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5703125" style="32" customWidth="1" collapsed="1"/>
-    <col min="16" max="28" width="9.140625" style="32" collapsed="1"/>
-    <col min="29" max="29" width="12.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="30" max="38" width="9.140625" style="32" collapsed="1"/>
-    <col min="39" max="39" width="18.5703125" style="32" customWidth="1" collapsed="1"/>
-    <col min="40" max="16384" width="9.140625" style="32" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="32" width="17.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="32" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="32" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="32" width="18.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="32" width="21.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="32" width="24.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="32" width="21.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="32" width="18.0" collapsed="true"/>
+    <col min="9" max="9" style="32" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="32" width="31.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="32" width="12.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="32" width="10.85546875" collapsed="true"/>
+    <col min="13" max="13" style="32" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="32" width="12.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="32" width="15.5703125" collapsed="true"/>
+    <col min="16" max="28" style="32" width="9.140625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="32" width="12.7109375" collapsed="true"/>
+    <col min="30" max="38" style="32" width="9.140625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" style="32" width="18.5703125" collapsed="true"/>
+    <col min="40" max="16384" style="32" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
@@ -11976,26 +12000,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" style="17" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" style="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="17" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="9.140625" style="17" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="9.140625" style="17" collapsed="1"/>
-    <col min="18" max="18" width="9.85546875" style="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="36.5703125" style="17" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.28515625" style="17" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="16.42578125" style="17" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="15.140625" style="17" customWidth="1" collapsed="1"/>
-    <col min="23" max="16384" width="9.140625" style="17" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="17" width="23.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="17" width="19.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="17" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="17" width="24.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="17" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="17" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="17" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="17" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="17" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="17" width="15.140625" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="17" width="14.42578125" collapsed="true"/>
+    <col min="13" max="14" style="17" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="17" width="13.140625" collapsed="true"/>
+    <col min="16" max="17" style="17" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="17" width="9.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="17" width="36.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="17" width="14.28515625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="17" width="16.42578125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="17" width="15.140625" collapsed="true"/>
+    <col min="23" max="16384" style="17" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
@@ -12326,13 +12350,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="18.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
@@ -12650,49 +12674,49 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="23" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="9.140625" collapsed="1"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.140625" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="23" width="9.140625" collapsed="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="27" width="9.140625" collapsed="1"/>
-    <col min="28" max="28" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="26.85546875" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="16" customWidth="1" collapsed="1"/>
-    <col min="33" max="37" width="9.140625" collapsed="1"/>
-    <col min="38" max="38" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="51" width="9.140625" collapsed="1"/>
-    <col min="52" max="52" width="23" customWidth="1" collapsed="1"/>
-    <col min="53" max="56" width="9.140625" collapsed="1"/>
-    <col min="57" max="57" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="58" max="61" width="9.140625" collapsed="1"/>
-    <col min="62" max="62" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="64" max="65" width="9.140625" collapsed="1"/>
-    <col min="66" max="66" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="20.42578125" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="70" max="70" width="9.140625" collapsed="1"/>
-    <col min="71" max="71" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="73" max="16384" width="9.140625" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="11" max="12" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="14" max="14" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="17" max="23" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="25" max="27" width="9.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="26.85546875" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="33" max="37" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="42" max="51" width="9.140625" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="53" max="56" width="9.140625" collapsed="true"/>
+    <col min="57" max="57" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="58" max="61" width="9.140625" collapsed="true"/>
+    <col min="62" max="62" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="63" max="63" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="64" max="65" width="9.140625" collapsed="true"/>
+    <col min="66" max="66" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="69" max="69" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="70" max="70" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="73" max="16384" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15.75" x14ac:dyDescent="0.25">
@@ -13871,7 +13895,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -13931,22 +13955,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.140625" style="35" collapsed="1"/>
-    <col min="3" max="3" width="19.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" style="35" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.5703125" style="35" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="35" collapsed="1"/>
-    <col min="10" max="10" width="23.5703125" style="35" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="9.140625" style="35" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.140625" style="35" customWidth="1" collapsed="1"/>
-    <col min="17" max="23" width="9.140625" style="35" collapsed="1"/>
-    <col min="24" max="24" width="12.42578125" style="35" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="20.85546875" style="35" customWidth="1" collapsed="1"/>
-    <col min="26" max="16384" width="9.140625" style="35" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="35" width="14.0" collapsed="true"/>
+    <col min="2" max="2" style="35" width="9.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="35" width="19.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="35" width="20.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="35" width="17.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="35" width="20.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="35" width="16.5703125" collapsed="true"/>
+    <col min="8" max="9" style="35" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="35" width="23.5703125" collapsed="true"/>
+    <col min="11" max="14" style="35" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="35" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="35" width="13.140625" collapsed="true"/>
+    <col min="17" max="23" style="35" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="35" width="12.42578125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="35" width="20.85546875" collapsed="true"/>
+    <col min="26" max="16384" style="35" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
@@ -14315,23 +14339,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="1" collapsed="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="25.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="9.140625" style="1" collapsed="1"/>
-    <col min="10" max="10" width="27.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="14" width="9.140625" style="1" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="22" width="9.140625" style="1" collapsed="1"/>
-    <col min="23" max="23" width="11.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="22" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="14.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="25.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
+    <col min="8" max="9" style="1" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="27.42578125" collapsed="true"/>
+    <col min="11" max="14" style="1" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="18" max="22" style="1" width="9.140625" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="22.0" collapsed="true"/>
+    <col min="25" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
@@ -14652,31 +14676,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="142" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" style="142" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" style="142" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="142" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" style="142" customWidth="1" collapsed="1"/>
-    <col min="6" max="13" width="9.140625" style="142" collapsed="1"/>
-    <col min="14" max="14" width="14.140625" style="142" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="9.140625" style="142" collapsed="1"/>
-    <col min="17" max="17" width="15.7109375" style="142" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="9.140625" style="142" collapsed="1"/>
-    <col min="19" max="19" width="13.140625" style="142" customWidth="1" collapsed="1"/>
-    <col min="20" max="23" width="9.140625" style="142" collapsed="1"/>
-    <col min="24" max="24" width="23.7109375" style="142" customWidth="1" collapsed="1"/>
-    <col min="25" max="26" width="9.140625" style="142" collapsed="1"/>
-    <col min="27" max="27" width="16.42578125" style="142" customWidth="1" collapsed="1"/>
-    <col min="28" max="45" width="9.140625" style="142" collapsed="1"/>
-    <col min="46" max="46" width="28.5703125" style="142" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="13.5703125" style="142" customWidth="1" collapsed="1"/>
-    <col min="48" max="64" width="9.140625" style="142" collapsed="1"/>
-    <col min="65" max="65" width="19.7109375" style="142" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="9.140625" style="142" collapsed="1"/>
-    <col min="67" max="67" width="17.28515625" style="142" customWidth="1" collapsed="1"/>
-    <col min="68" max="70" width="9.140625" style="142" collapsed="1"/>
-    <col min="71" max="71" width="15.7109375" style="142" customWidth="1" collapsed="1"/>
-    <col min="72" max="16384" width="9.140625" style="142" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="142" width="15.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="142" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="142" width="18.0" collapsed="true"/>
+    <col min="4" max="4" style="142" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="142" width="20.140625" collapsed="true"/>
+    <col min="6" max="13" style="142" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="142" width="14.140625" collapsed="true"/>
+    <col min="15" max="16" style="142" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="142" width="15.7109375" collapsed="true"/>
+    <col min="18" max="18" style="142" width="9.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="142" width="13.140625" collapsed="true"/>
+    <col min="20" max="23" style="142" width="9.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="142" width="23.7109375" collapsed="true"/>
+    <col min="25" max="26" style="142" width="9.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="142" width="16.42578125" collapsed="true"/>
+    <col min="28" max="45" style="142" width="9.140625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="142" width="28.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="142" width="13.5703125" collapsed="true"/>
+    <col min="48" max="64" style="142" width="9.140625" collapsed="true"/>
+    <col min="65" max="65" customWidth="true" style="142" width="19.7109375" collapsed="true"/>
+    <col min="66" max="66" style="142" width="9.140625" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" style="142" width="17.28515625" collapsed="true"/>
+    <col min="68" max="70" style="142" width="9.140625" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" style="142" width="15.7109375" collapsed="true"/>
+    <col min="72" max="16384" style="142" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.25">
@@ -16800,8 +16824,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="20.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17616,60 +17640,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" style="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24" style="26" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" style="26" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="56.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="11" max="12" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.140625" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.140625" style="26" collapsed="1"/>
-    <col min="17" max="17" width="16.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.42578125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="12.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="17.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="23.140625" style="26" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="16.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="16" style="26" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="28.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="19.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="29.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="21.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="41.7109375" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="38.42578125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.42578125" style="72" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="40" width="9.140625" style="26" collapsed="1"/>
-    <col min="41" max="41" width="27.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="9.140625" collapsed="1"/>
-    <col min="43" max="43" width="20.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="13.5703125" style="26" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="39.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="12.5703125" style="26" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="19.7109375" style="26" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="14.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="49" max="50" width="21.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="18" style="26" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="20.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="22.42578125" style="26" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="20.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="17.85546875" style="26" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="19.28515625" style="26" customWidth="1" collapsed="1"/>
-    <col min="57" max="16384" width="9.140625" style="26" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="26" width="25.9140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="26" width="14.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="26" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="26" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="26" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="26" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" style="26" width="9.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="26" width="18.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="26" width="56.7109375" collapsed="true"/>
+    <col min="11" max="12" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="26" width="14.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="26" width="20.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="26" width="13.140625" collapsed="true"/>
+    <col min="16" max="16" style="26" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="26" width="16.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="26" width="24.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="26" width="12.484375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="26" width="12.85546875" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="26" width="17.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="26" width="11.85546875" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="26" width="15.28515625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="26" width="23.140625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="26" width="16.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="26" width="16.0" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="26" width="28.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="26" width="19.7109375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="26" width="22.28515625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="26" width="29.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="26" width="21.7109375" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="41.7109375" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" style="72" width="12.42578125" collapsed="true"/>
+    <col min="39" max="40" style="26" width="9.140625" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" style="26" width="27.7109375" collapsed="true"/>
+    <col min="42" max="42" width="9.140625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="26" width="20.7109375" collapsed="true"/>
+    <col min="44" max="44" bestFit="true" customWidth="true" style="26" width="13.5703125" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" style="26" width="39.28515625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" style="26" width="12.5703125" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" style="26" width="19.7109375" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="26" width="14.42578125" collapsed="true"/>
+    <col min="49" max="50" customWidth="true" style="26" width="21.85546875" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" style="26" width="18.0" collapsed="true"/>
+    <col min="52" max="52" customWidth="true" style="26" width="20.42578125" collapsed="true"/>
+    <col min="53" max="53" customWidth="true" style="26" width="22.42578125" collapsed="true"/>
+    <col min="54" max="54" customWidth="true" style="26" width="20.85546875" collapsed="true"/>
+    <col min="55" max="55" customWidth="true" style="26" width="17.85546875" collapsed="true"/>
+    <col min="56" max="56" customWidth="true" style="26" width="19.28515625" collapsed="true"/>
+    <col min="57" max="16384" style="26" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
@@ -17844,7 +17868,7 @@
     </row>
     <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>1136</v>
+        <v>1144</v>
       </c>
       <c r="B2" s="26" t="s">
         <v>360</v>
@@ -18014,7 +18038,7 @@
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>385</v>
+        <v>1145</v>
       </c>
       <c r="B3" s="26" t="s">
         <v>360</v>
@@ -18061,7 +18085,7 @@
         <v>391</v>
       </c>
       <c r="U3" s="58" t="s">
-        <v>392</v>
+        <v>1146</v>
       </c>
       <c r="V3" s="58" t="s">
         <v>267</v>
@@ -18411,55 +18435,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="18" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="29.140625" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="21" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="26.5703125" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="28.42578125" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="40.85546875" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="20.85546875" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="19" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="23.42578125" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.19140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="12.09765625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="28.42578125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="40.85546875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="12.4296875" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="40" max="40" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="41" max="41" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" width="20.85546875" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="44" max="44" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="45" max="45" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="46" max="46" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="47" max="47" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
@@ -18762,7 +18786,7 @@
     </row>
     <row r="3" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>431</v>
+        <v>1139</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>419</v>
@@ -18810,7 +18834,7 @@
         <v>369</v>
       </c>
       <c r="U3" s="58" t="s">
-        <v>436</v>
+        <v>1141</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>267</v>
@@ -18858,7 +18882,7 @@
         <v>92</v>
       </c>
       <c r="AK3" s="29" t="s">
-        <v>439</v>
+        <v>1138</v>
       </c>
       <c r="AL3" s="26" t="s">
         <v>126</v>
@@ -19074,22 +19098,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="15.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="15.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="11.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.140625" style="1" collapsed="1"/>
-    <col min="14" max="14" width="15.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="12.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="23.140625" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="4" max="6" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="30.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="21.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="13" max="13" style="1" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="1" width="15.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="12.140625" collapsed="true"/>
+    <col min="19" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -19630,10 +19654,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -19722,37 +19746,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.140625" collapsed="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.140625" collapsed="1"/>
-    <col min="15" max="15" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="19" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="16" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="35.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" width="9.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="14" max="14" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="16" max="17" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="37" max="37" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -20384,29 +20408,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="29" width="9.140625" style="1" collapsed="1"/>
-    <col min="30" max="30" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="17.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="20.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="24.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="26" style="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="18.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="37" width="9.140625" style="1" collapsed="1"/>
-    <col min="38" max="38" width="13.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="41" width="9.140625" style="1" collapsed="1"/>
-    <col min="42" max="42" width="15.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="13" style="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="17.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="11" max="29" style="1" width="9.140625" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
+    <col min="31" max="31" customWidth="true" style="1" width="17.7109375" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="1" width="20.140625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" style="1" width="26.0" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
+    <col min="36" max="37" style="1" width="9.140625" collapsed="true"/>
+    <col min="38" max="38" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="39" max="41" style="1" width="9.140625" collapsed="true"/>
+    <col min="42" max="42" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="44" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
City/comm local angular wait changes
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
+++ b/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34BD50E-A590-483E-B679-5E0651568E2F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFACECB-5893-482A-97C4-920611CCFB27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4250,7 +4250,7 @@
     <t>1000089389</t>
   </si>
   <si>
-    <t>1000167570</t>
+    <t>1000167435</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
TUG and LEED Cities
</commit_message>
<xml_diff>
--- a/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
+++ b/AutomationArc/ARCDataTemplete/QasArcTest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AutomationArc\AutomationArc\ARCDataTemplete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationArc\AutomationArc\AutomationArc\ARCDataTemplete\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A95AFE-6823-4DD2-B616-46C2E6A110B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USBuildingProject" sheetId="1" r:id="rId1"/>
@@ -41,17 +42,12 @@
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5533" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5545" uniqueCount="1394">
   <si>
     <t>ProjectName</t>
   </si>
@@ -4219,27 +4215,30 @@
     <t>Jun 26, 2019</t>
   </si>
   <si>
-    <t>1000167461</t>
-  </si>
-  <si>
     <t>1000167902</t>
   </si>
   <si>
-    <t>MySchools</t>
-  </si>
-  <si>
     <t>1000167885</t>
   </si>
   <si>
     <t>USTransitAbovegroundSuite</t>
+  </si>
+  <si>
+    <t>1000089836</t>
+  </si>
+  <si>
+    <t>USBuildingNoneSuite</t>
+  </si>
+  <si>
+    <t>https://qas.app.arconline.io/app/project/1000089836/survey/v2/?key=EK6JPVqtvulMvPBgxcpgdg0K&amp;language=en</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -4765,8 +4764,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="11" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4869,8 +4868,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="8" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4912,19 +4911,19 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="8" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5265,11 +5264,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5584,7 +5583,7 @@
         <v>80</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
@@ -5731,7 +5730,7 @@
         <v>101</v>
       </c>
       <c r="O3" s="58" t="s">
-        <v>1391</v>
+        <v>1389</v>
       </c>
       <c r="P3" t="s">
         <v>102</v>
@@ -6189,7 +6188,7 @@
         <v>101</v>
       </c>
       <c r="O6" s="58" t="s">
-        <v>1388</v>
+        <v>1391</v>
       </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
@@ -6537,7 +6536,7 @@
         <v>193</v>
       </c>
       <c r="O11" s="58" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
@@ -6664,7 +6663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AN10"/>
   <sheetViews>
     <sheetView topLeftCell="D5" workbookViewId="0">
@@ -7326,7 +7325,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AQ5"/>
   <sheetViews>
     <sheetView topLeftCell="B18" workbookViewId="0">
@@ -7993,7 +7992,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:BU15"/>
   <sheetViews>
     <sheetView topLeftCell="BM1" zoomScaleNormal="100" workbookViewId="0">
@@ -9694,7 +9693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:BT15"/>
   <sheetViews>
     <sheetView topLeftCell="BJ1" workbookViewId="0">
@@ -11361,7 +11360,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
@@ -11685,16 +11684,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView topLeftCell="Q1" workbookViewId="0">
@@ -12034,9 +12033,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0E00-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0E00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -12044,7 +12043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -12338,16 +12337,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="M3" r:id="rId4"/>
-    <hyperlink ref="D4" r:id="rId5"/>
-    <hyperlink ref="M4" r:id="rId6"/>
-    <hyperlink ref="D5" r:id="rId7"/>
-    <hyperlink ref="M5" r:id="rId8"/>
-    <hyperlink ref="D6" r:id="rId9"/>
-    <hyperlink ref="M6" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="M3" r:id="rId4" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="M4" r:id="rId6" xr:uid="{00000000-0004-0000-0F00-000005000000}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{00000000-0004-0000-0F00-000006000000}"/>
+    <hyperlink ref="M5" r:id="rId8" xr:uid="{00000000-0004-0000-0F00-000007000000}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{00000000-0004-0000-0F00-000008000000}"/>
+    <hyperlink ref="M6" r:id="rId10" xr:uid="{00000000-0004-0000-0F00-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
@@ -12355,7 +12354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AO10"/>
   <sheetViews>
     <sheetView topLeftCell="AE1" workbookViewId="0">
@@ -13018,7 +13017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView topLeftCell="R1" workbookViewId="0">
@@ -13359,16 +13358,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-1100-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-1100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
@@ -13683,16 +13682,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-1200-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BT13"/>
   <sheetViews>
     <sheetView topLeftCell="S2" workbookViewId="0">
@@ -14915,7 +14914,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:AL5"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
@@ -15401,16 +15400,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-1300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:BT15"/>
   <sheetViews>
     <sheetView topLeftCell="BD1" workbookViewId="0">
@@ -16620,7 +16619,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
@@ -16948,16 +16947,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-1500-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:BT28"/>
   <sheetViews>
     <sheetView topLeftCell="BJ1" workbookViewId="0">
@@ -19108,7 +19107,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -19157,18 +19156,18 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A6" r:id="rId2"/>
-    <hyperlink ref="A7" r:id="rId3"/>
-    <hyperlink ref="A2" r:id="rId4"/>
-    <hyperlink ref="A3:A4" r:id="rId5" display="qas-02@gmail.com"/>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A6" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A7" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A3:A4" r:id="rId5" display="qas-02@gmail.com" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView topLeftCell="I1" workbookViewId="0">
@@ -20044,7 +20043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:CE20"/>
   <sheetViews>
     <sheetView topLeftCell="BL1" workbookViewId="0">
@@ -24020,9 +24019,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -24030,7 +24029,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BU15"/>
   <sheetViews>
     <sheetView topLeftCell="BM1" workbookViewId="0">
@@ -24044,14 +24043,14 @@
     <col min="62" max="62" customWidth="true" width="15.140625" collapsed="true"/>
     <col min="63" max="63" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="64" max="64" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="101.42578125" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="103.9765625" collapsed="true"/>
     <col min="66" max="66" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="67" max="67" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="68" max="68" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
     <col min="69" max="69" customWidth="true" width="13.5703125" collapsed="true"/>
     <col min="70" max="70" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="71" max="71" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="14.08984375" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="19.82421875" collapsed="true"/>
     <col min="73" max="73" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
@@ -24464,7 +24463,7 @@
         <v>829</v>
       </c>
       <c r="BM2" s="120" t="s">
-        <v>830</v>
+        <v>1393</v>
       </c>
       <c r="BN2" s="116" t="s">
         <v>831</v>
@@ -25324,14 +25323,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BM2" r:id="rId1"/>
+    <hyperlink ref="BM2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AW7"/>
   <sheetViews>
     <sheetView topLeftCell="AV1" workbookViewId="0">
@@ -25984,9 +25983,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -25994,7 +25993,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26537,12 +26536,12 @@
     <cfRule type="uniqueValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3:H6" r:id="rId2" display="usgbcarc@gmail.com"/>
-    <hyperlink ref="H7" r:id="rId3"/>
-    <hyperlink ref="H8" r:id="rId4"/>
-    <hyperlink ref="H10" r:id="rId5"/>
-    <hyperlink ref="H9" r:id="rId6"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="H3:H6" r:id="rId2" display="usgbcarc@gmail.com" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="H7" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="H8" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="H10" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -26550,7 +26549,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>